<commit_message>
comments and cleaning up
</commit_message>
<xml_diff>
--- a/flesh_detection/test_labels.xlsx
+++ b/flesh_detection/test_labels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\palle\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0CCF776-D00E-473F-8850-DCEA5349507E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058C2382-47C6-47DD-A274-D23B2D738C19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8172" yWindow="348" windowWidth="12528" windowHeight="8964" xr2:uid="{89D94C57-F344-4DDD-BAC8-8CE43354AE34}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{89D94C57-F344-4DDD-BAC8-8CE43354AE34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D71117D-B725-4C05-AAE6-4B2909B3C48B}">
-  <dimension ref="A1:D463"/>
+  <dimension ref="A1:D464"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A445" workbookViewId="0">
-      <selection activeCell="H462" sqref="H462"/>
+      <selection activeCell="G464" sqref="G464"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4136,6 +4136,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A464">
+        <v>463</v>
+      </c>
+      <c r="B464">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>